<commit_message>
Changed first 3 changes from index.md
</commit_message>
<xml_diff>
--- a/Script/data/CodeExcel.xlsx
+++ b/Script/data/CodeExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S530473\Desktop\GDP1\Project-Charter-Group-D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531500\Desktop\New folder\Project-Charter-Group-D\Script\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{480C9374-DB6A-42E7-A9B2-A81BBF843A57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02B4CBBA-D5C5-4E7B-B9F8-48FD54012C64}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{B22338A6-5A6F-4A97-976D-53EBE18763A7}"/>
   </bookViews>
@@ -715,7 +715,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B97F6B-761F-4606-AB72-71E475E30B14}">
   <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1602,9 +1604,9 @@
       </c>
     </row>
     <row r="89" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="e">
-        <f>Codeword!D1:V2=B91=+CodwordSet!$A$2</f>
-        <v>#VALUE!</v>
+      <c r="A89" s="3" t="str">
+        <f>+CodwordSet!$A$2</f>
+        <v>Hoot 96</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>87</v>

</xml_diff>